<commit_message>
Choleksy decomposition for symmetric matrices
</commit_message>
<xml_diff>
--- a/jacobi/src/test/resources/jacobi/test/data/CholeskyDecompTest.xlsx
+++ b/jacobi/src/test/resources/jacobi/test/data/CholeskyDecompTest.xlsx
@@ -4,31 +4,38 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="21075" windowHeight="8250" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="21075" windowHeight="8250" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="3x3" sheetId="1" r:id="rId1"/>
     <sheet name="4x4" sheetId="2" r:id="rId2"/>
-    <sheet name="rand" sheetId="3" r:id="rId3"/>
+    <sheet name="Symmetric 5x5" sheetId="4" r:id="rId3"/>
+    <sheet name="rand" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
   <si>
     <t>#1</t>
   </si>
   <si>
     <t>#2</t>
   </si>
+  <si>
+    <t>L=</t>
+  </si>
+  <si>
+    <t>L*L^t=</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -36,13 +43,50 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -54,13 +98,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
+    <cellStyle name="20% - Accent1" xfId="3" builtinId="30"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -497,7 +550,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10:D13"/>
     </sheetView>
   </sheetViews>
@@ -702,10 +755,395 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>0.17074494559074171</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <f t="array" ref="G2:K6">TRANSPOSE(A2:E6)</f>
+        <v>0.17074494559074171</v>
+      </c>
+      <c r="H2">
+        <v>-0.83198829529416662</v>
+      </c>
+      <c r="I2" s="1">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>-0.83198829529416662</v>
+      </c>
+      <c r="B3" s="1">
+        <v>4.329846413723093E-2</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>4.329846413723093E-2</v>
+      </c>
+      <c r="I3" s="1">
+        <v>-0.92562597535406388</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4" s="3">
+        <v>-0.92562597535406388</v>
+      </c>
+      <c r="C4" s="2">
+        <v>-0.61126889464138534</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4" s="1">
+        <v>-0.61126889464138534</v>
+      </c>
+      <c r="J4">
+        <v>-0.37217123934736018</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5" s="3">
+        <v>-0.37217123934736018</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.28571318300644588</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5" s="1">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0.28571318300644588</v>
+      </c>
+      <c r="K5">
+        <v>0.47110628815187305</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0.47110628815187305</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.41980490194444364</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6" s="1">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0.41980490194444364</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <f>A2*A2</f>
+        <v>2.915383644478535E-2</v>
+      </c>
+      <c r="B10" s="3">
+        <f>A3*A3</f>
+        <v>0.69220452350649342</v>
+      </c>
+      <c r="C10" s="2">
+        <f>B3*B3</f>
+        <v>1.874756996643073E-3</v>
+      </c>
+      <c r="D10" s="3">
+        <f>B4*B4</f>
+        <v>0.85678344625016212</v>
+      </c>
+      <c r="E10" s="2">
+        <f>C4*C4</f>
+        <v>0.37364966155610108</v>
+      </c>
+      <c r="F10" s="3">
+        <f>C5*C5</f>
+        <v>0.13851143139735006</v>
+      </c>
+      <c r="G10" s="2">
+        <f>D5*D5</f>
+        <v>8.1632022943674831E-2</v>
+      </c>
+      <c r="H10" s="3">
+        <f>D6*D6</f>
+        <v>0.22194113473623564</v>
+      </c>
+      <c r="I10" s="2">
+        <f>E6*E6</f>
+        <v>0.17623615569658393</v>
+      </c>
+      <c r="J10" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <f t="array" ref="A13:E17">MMULT(A2:E6,TRANSPOSE(A2:E6))</f>
+        <v>2.915383644478535E-2</v>
+      </c>
+      <c r="B13" s="3">
+        <v>-0.14205779621213643</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <f>B14-B10</f>
+        <v>1.8747569966430788E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>-0.14205779621213643</v>
+      </c>
+      <c r="B14" s="2">
+        <v>0.6940792805031365</v>
+      </c>
+      <c r="C14" s="3">
+        <v>-4.0078183098357333E-2</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>0</v>
+      </c>
+      <c r="B15">
+        <v>-4.0078183098357333E-2</v>
+      </c>
+      <c r="C15" s="2">
+        <v>1.2304331078062631</v>
+      </c>
+      <c r="D15" s="3">
+        <v>0.22749670209317532</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>0</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>0.22749670209317532</v>
+      </c>
+      <c r="D16" s="2">
+        <v>0.22014345434102489</v>
+      </c>
+      <c r="E16" s="3">
+        <v>0.13460127712222353</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>0</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0.13460127712222353</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0.39817729043281958</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <f>A13</f>
+        <v>2.915383644478535E-2</v>
+      </c>
+      <c r="B21" s="3">
+        <f>B13</f>
+        <v>-0.14205779621213643</v>
+      </c>
+      <c r="C21" s="2">
+        <f>B14</f>
+        <v>0.6940792805031365</v>
+      </c>
+      <c r="D21" s="3">
+        <f>C14</f>
+        <v>-4.0078183098357333E-2</v>
+      </c>
+      <c r="E21" s="2">
+        <f>C15</f>
+        <v>1.2304331078062631</v>
+      </c>
+      <c r="F21" s="3">
+        <f>D15</f>
+        <v>0.22749670209317532</v>
+      </c>
+      <c r="G21" s="2">
+        <f>D16</f>
+        <v>0.22014345434102489</v>
+      </c>
+      <c r="H21" s="3">
+        <f>E16</f>
+        <v>0.13460127712222353</v>
+      </c>
+      <c r="I21" s="2">
+        <f>E17</f>
+        <v>0.39817729043281958</v>
+      </c>
+      <c r="J21" s="1">
+        <f>F17</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D4"/>
+      <selection activeCell="F11" sqref="B7:F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -713,901 +1151,901 @@
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1">
         <f ca="1">RAND() * 2 - 1</f>
-        <v>8.5986137125549034E-2</v>
+        <v>-0.28827794836252862</v>
       </c>
       <c r="B1">
         <f t="shared" ref="B1:G16" ca="1" si="0">RAND() * 2 - 1</f>
-        <v>-0.31400586361111671</v>
+        <v>0.58383275438160465</v>
       </c>
       <c r="C1">
         <f t="shared" ca="1" si="0"/>
-        <v>0.71570476661044324</v>
+        <v>0.77371185505554241</v>
       </c>
       <c r="D1">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.76019557939928628</v>
+        <v>0.87199893457261601</v>
       </c>
       <c r="E1">
         <f t="shared" ca="1" si="0"/>
-        <v>0.83145690524970739</v>
+        <v>0.34244472729494979</v>
       </c>
       <c r="F1">
         <f t="shared" ca="1" si="0"/>
-        <v>0.31974034990193423</v>
+        <v>-0.46674622912542585</v>
       </c>
       <c r="G1">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.22699097352894815</v>
+        <v>0.94159990774756519</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <f t="shared" ref="A2:G30" ca="1" si="1">RAND() * 2 - 1</f>
-        <v>0.29819947696545124</v>
+        <v>0.34729668150576631</v>
       </c>
       <c r="B2">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.47842011077380686</v>
+        <v>-0.88586884983261038</v>
       </c>
       <c r="C2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.82807763910747356</v>
+        <v>0.80924232516687966</v>
       </c>
       <c r="D2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.19792073299860102</v>
+        <v>-0.57106136571804589</v>
       </c>
       <c r="E2">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.1547607797343542</v>
+        <v>0.22889426400265589</v>
       </c>
       <c r="F2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.11714198580369684</v>
+        <v>-0.45396856338372182</v>
       </c>
       <c r="G2">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.94346360468220603</v>
+        <v>0.2235635497053714</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <f t="shared" ca="1" si="1"/>
-        <v>0.49669440174314961</v>
+        <v>0.95045363582672682</v>
       </c>
       <c r="B3">
         <f t="shared" ca="1" si="0"/>
-        <v>9.3263344632388057E-2</v>
+        <v>-0.55543422940032583</v>
       </c>
       <c r="C3">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.89930144212155927</v>
+        <v>-0.97478165579579734</v>
       </c>
       <c r="D3">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.79644270390173788</v>
+        <v>-0.22742156030524163</v>
       </c>
       <c r="E3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.81410955622064529</v>
+        <v>-0.15146467730189328</v>
       </c>
       <c r="F3">
         <f t="shared" ca="1" si="0"/>
-        <v>6.0785670300503192E-2</v>
+        <v>0.12330256826293939</v>
       </c>
       <c r="G3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.21355280826419842</v>
+        <v>0.7270907726560496</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" ca="1" si="1"/>
-        <v>0.35784155702942133</v>
+        <v>0.32547297400936603</v>
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.18612939531886585</v>
+        <v>-0.52192705224867297</v>
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.17324687712374853</v>
+        <v>0.69237574279456182</v>
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="0"/>
-        <v>-9.286738793323468E-2</v>
+        <v>0.75483808542886455</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.40627800509862388</v>
+        <v>0.11554472993404463</v>
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.49230436766888097</v>
+        <v>-0.80451587479452491</v>
       </c>
       <c r="G4">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.65301883946812</v>
+        <v>-0.69054411751569145</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.90827657193761824</v>
+        <v>0.44169196954915857</v>
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.18663970662554052</v>
+        <v>3.7259346502125368E-3</v>
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="0"/>
-        <v>3.7947069488917906E-2</v>
+        <v>5.9275923724066537E-2</v>
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.16154387684539229</v>
+        <v>-0.29282504713774937</v>
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.43873464258667694</v>
+        <v>0.36831299216686331</v>
       </c>
       <c r="F5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.18711636923999597</v>
+        <v>0.24122431794396948</v>
       </c>
       <c r="G5">
         <f t="shared" ca="1" si="0"/>
-        <v>5.2804547860378026E-2</v>
+        <v>-9.9164534208517008E-2</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" ca="1" si="1"/>
-        <v>0.19403868829559601</v>
+        <v>-0.55026928899280358</v>
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="0"/>
-        <v>0.18379336021669834</v>
+        <v>0.54830136136127039</v>
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.5163727713569219E-2</v>
+        <v>-0.65509974859752917</v>
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="0"/>
-        <v>0.79806283517201204</v>
+        <v>0.12915939083989203</v>
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="0"/>
-        <v>0.15192439575103722</v>
+        <v>-0.993295060588544</v>
       </c>
       <c r="F6">
         <f t="shared" ca="1" si="0"/>
-        <v>0.5798046305480582</v>
+        <v>-0.84478141321903899</v>
       </c>
       <c r="G6">
         <f t="shared" ca="1" si="0"/>
-        <v>0.40287870930777792</v>
+        <v>0.139400949608665</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.14675564810085051</v>
+        <v>0.74544724225521719</v>
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="0"/>
-        <v>0.81584338702555814</v>
+        <v>-0.34634718081749361</v>
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="0"/>
-        <v>0.12195422711855408</v>
+        <v>-6.6006461378494308E-2</v>
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="0"/>
-        <v>0.48637171939073975</v>
+        <v>4.9469248904318697E-2</v>
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="0"/>
-        <v>0.76596012481298348</v>
+        <v>-0.71051720137912033</v>
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.86654014339809127</v>
+        <v>0.37107919388900501</v>
       </c>
       <c r="G7">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.38612128101080256</v>
+        <v>-0.88202033998335305</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" ca="1" si="1"/>
-        <v>0.78510577046054286</v>
+        <v>0.93670291503615699</v>
       </c>
       <c r="B8">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.95862841098696405</v>
+        <v>0.32925305394598303</v>
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="0"/>
-        <v>-6.6444648604500056E-2</v>
+        <v>0.85593508793013529</v>
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.87343601092640966</v>
+        <v>-0.35183360540386732</v>
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.84532313524258429</v>
+        <v>-0.51264762781939077</v>
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.63385031975392669</v>
+        <v>0.8003163144093266</v>
       </c>
       <c r="G8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.13599706110550613</v>
+        <v>-0.17687262967163009</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" ca="1" si="1"/>
-        <v>0.2046736328103822</v>
+        <v>0.10472827268319262</v>
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="0"/>
-        <v>0.83906555363147484</v>
+        <v>-0.51853680385041634</v>
       </c>
       <c r="C9">
         <f t="shared" ca="1" si="0"/>
-        <v>0.61068660255675722</v>
+        <v>-0.29958206984635005</v>
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.75390992078768959</v>
+        <v>-0.30907060481023074</v>
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.51987581318441412</v>
+        <v>0.63404928625632895</v>
       </c>
       <c r="F9">
         <f t="shared" ca="1" si="0"/>
-        <v>-6.6405660966848412E-2</v>
+        <v>-0.17157278470340764</v>
       </c>
       <c r="G9">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.48112199370873454</v>
+        <v>0.87289902853880874</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.8697222421883346</v>
+        <v>-0.36706776163176014</v>
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.87558269650696219</v>
+        <v>-0.87988127051796794</v>
       </c>
       <c r="C10">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.14376793609860483</v>
+        <v>0.55044276553135707</v>
       </c>
       <c r="D10">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.75907200986074641</v>
+        <v>-0.64919696323804521</v>
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.1420478122467168E-2</v>
+        <v>-0.9742418233423642</v>
       </c>
       <c r="F10">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.50351615923363346</v>
+        <v>-1.7073713385855616E-2</v>
       </c>
       <c r="G10">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.40331054987392956</v>
+        <v>-0.26642928963049606</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.85722883972111297</v>
+        <v>5.8965267769937046E-2</v>
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="0"/>
-        <v>0.90781981256396538</v>
+        <v>0.86739962433803508</v>
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="0"/>
-        <v>0.83266577216057391</v>
+        <v>-0.35974240038528094</v>
       </c>
       <c r="D11">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.93916162697664718</v>
+        <v>0.1221156445763103</v>
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.17660867011062864</v>
+        <v>0.71458466479372129</v>
       </c>
       <c r="F11">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.16316544334970362</v>
+        <v>0.70068973979563309</v>
       </c>
       <c r="G11">
         <f t="shared" ca="1" si="0"/>
-        <v>0.88517262880716974</v>
+        <v>0.54344673322275461</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.71797840427220927</v>
+        <v>-0.41329117299175944</v>
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="0"/>
-        <v>0.87682127743309457</v>
+        <v>-0.37121145710261483</v>
       </c>
       <c r="C12">
         <f t="shared" ca="1" si="0"/>
-        <v>0.84351888932294372</v>
+        <v>-0.18266415534245173</v>
       </c>
       <c r="D12">
         <f t="shared" ca="1" si="0"/>
-        <v>0.15219918748778971</v>
+        <v>0.86848810456528946</v>
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="0"/>
-        <v>0.21836174371866179</v>
+        <v>-0.45724755895818858</v>
       </c>
       <c r="F12">
         <f t="shared" ca="1" si="0"/>
-        <v>0.87743230121452354</v>
+        <v>0.42344330929109963</v>
       </c>
       <c r="G12">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.35223116357128048</v>
+        <v>-0.87572955268722374</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.59622782114617356</v>
+        <v>0.91499120820015745</v>
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.98042977952254762</v>
+        <v>-0.67947198094070482</v>
       </c>
       <c r="C13">
         <f t="shared" ca="1" si="0"/>
-        <v>0.37078457915805396</v>
+        <v>0.30187521380556537</v>
       </c>
       <c r="D13">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.92894742593877266</v>
+        <v>0.76574467516090228</v>
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.18193642561740964</v>
+        <v>0.10186951989214643</v>
       </c>
       <c r="F13">
         <f t="shared" ca="1" si="0"/>
-        <v>0.81996628226107049</v>
+        <v>-0.51255518845115011</v>
       </c>
       <c r="G13">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.77333008144134818</v>
+        <v>-0.93802283515883844</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" ca="1" si="1"/>
-        <v>0.58169346119410648</v>
+        <v>0.7114085511642676</v>
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.19719897508172024</v>
+        <v>0.41811826976859701</v>
       </c>
       <c r="C14">
         <f t="shared" ca="1" si="0"/>
-        <v>0.96285769290494394</v>
+        <v>-0.526866129681415</v>
       </c>
       <c r="D14">
         <f t="shared" ca="1" si="0"/>
-        <v>0.6467123730096711</v>
+        <v>0.34807879386903906</v>
       </c>
       <c r="E14">
         <f t="shared" ca="1" si="0"/>
-        <v>0.39075371198841236</v>
+        <v>0.97751987297172316</v>
       </c>
       <c r="F14">
         <f t="shared" ca="1" si="0"/>
-        <v>0.29452071446654737</v>
+        <v>-2.7076807967009175E-2</v>
       </c>
       <c r="G14">
         <f t="shared" ca="1" si="0"/>
-        <v>0.86266945362356706</v>
+        <v>0.4420717337586213</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.62278469299520611</v>
+        <v>-0.41303114195717328</v>
       </c>
       <c r="B15">
         <f t="shared" ca="1" si="0"/>
-        <v>0.4931633256297776</v>
+        <v>6.3143584541432762E-2</v>
       </c>
       <c r="C15">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.21935953254146301</v>
+        <v>0.12512870694459211</v>
       </c>
       <c r="D15">
         <f t="shared" ca="1" si="0"/>
-        <v>0.54524161325844367</v>
+        <v>-0.12068537445045102</v>
       </c>
       <c r="E15">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.95600911420382739</v>
+        <v>-0.60574419319606165</v>
       </c>
       <c r="F15">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.2338913249133987</v>
+        <v>0.16274066663440734</v>
       </c>
       <c r="G15">
         <f t="shared" ca="1" si="0"/>
-        <v>0.79653194748377865</v>
+        <v>-0.4458993884036353</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" ca="1" si="1"/>
-        <v>0.56093454021269462</v>
+        <v>-0.7277424459523778</v>
       </c>
       <c r="B16">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.1842913500733423</v>
+        <v>-0.31508291903698082</v>
       </c>
       <c r="C16">
         <f t="shared" ca="1" si="0"/>
-        <v>0.81946888088103198</v>
+        <v>0.97209229401808361</v>
       </c>
       <c r="D16">
         <f t="shared" ca="1" si="0"/>
-        <v>0.55981039793630893</v>
+        <v>-0.66002174093472599</v>
       </c>
       <c r="E16">
         <f t="shared" ca="1" si="0"/>
-        <v>0.82828681635441792</v>
+        <v>0.91960758283095534</v>
       </c>
       <c r="F16">
         <f t="shared" ca="1" si="0"/>
-        <v>0.61324828154844435</v>
+        <v>-0.17532121295054681</v>
       </c>
       <c r="G16">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.28255090695904705</v>
+        <v>-0.89313903936592287</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" ca="1" si="1"/>
-        <v>0.72674577393127371</v>
+        <v>0.63381202744096266</v>
       </c>
       <c r="B17">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.64833211430886117</v>
+        <v>-0.32343282187481037</v>
       </c>
       <c r="C17">
         <f t="shared" ca="1" si="1"/>
-        <v>0.78687106332492651</v>
+        <v>0.87511906060171274</v>
       </c>
       <c r="D17">
         <f t="shared" ca="1" si="1"/>
-        <v>0.59889337473380833</v>
+        <v>-0.6926042686365943</v>
       </c>
       <c r="E17">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.8274030414278768</v>
+        <v>0.41950556626184499</v>
       </c>
       <c r="F17">
         <f t="shared" ca="1" si="1"/>
-        <v>0.21107248230143472</v>
+        <v>0.49799388473600281</v>
       </c>
       <c r="G17">
         <f t="shared" ca="1" si="1"/>
-        <v>-7.3490243935399269E-2</v>
+        <v>9.0453257236331686E-2</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" ca="1" si="1"/>
-        <v>0.69528356399391056</v>
+        <v>-0.6183956052588393</v>
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.24812729645782627</v>
+        <v>-0.39040244551659198</v>
       </c>
       <c r="C18">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.74461179278306022</v>
+        <v>0.158734529656259</v>
       </c>
       <c r="D18">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.52885985256301127</v>
+        <v>-9.2555523332074952E-2</v>
       </c>
       <c r="E18">
         <f t="shared" ca="1" si="1"/>
-        <v>0.58145153450408715</v>
+        <v>-0.9000412010304204</v>
       </c>
       <c r="F18">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.67914968280037535</v>
+        <v>0.73118315849307058</v>
       </c>
       <c r="G18">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.55265036244735422</v>
+        <v>1.1326349153659043E-2</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.17509951099494958</v>
+        <v>-0.9965187678704881</v>
       </c>
       <c r="B19">
         <f t="shared" ca="1" si="1"/>
-        <v>0.4726102850231837</v>
+        <v>0.30012383005275867</v>
       </c>
       <c r="C19">
         <f t="shared" ca="1" si="1"/>
-        <v>0.35291865896399943</v>
+        <v>-0.57858165566858721</v>
       </c>
       <c r="D19">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.77389417515673542</v>
+        <v>0.3999878217659476</v>
       </c>
       <c r="E19">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.1393652769806546</v>
+        <v>0.55953099706950593</v>
       </c>
       <c r="F19">
         <f t="shared" ca="1" si="1"/>
-        <v>0.97230232524644311</v>
+        <v>8.2922758321032353E-2</v>
       </c>
       <c r="G19">
         <f t="shared" ca="1" si="1"/>
-        <v>0.38256807818368022</v>
+        <v>-0.34635377452074279</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.9741086412774842</v>
+        <v>0.48115627822988882</v>
       </c>
       <c r="B20">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.71171005265849141</v>
+        <v>-0.12730828310463638</v>
       </c>
       <c r="C20">
         <f t="shared" ca="1" si="1"/>
-        <v>0.84536989822069697</v>
+        <v>0.83228806078243167</v>
       </c>
       <c r="D20">
         <f t="shared" ca="1" si="1"/>
-        <v>-7.706959319833917E-2</v>
+        <v>0.32102165479096323</v>
       </c>
       <c r="E20">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.34120061625674714</v>
+        <v>0.25997247148808644</v>
       </c>
       <c r="F20">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.59482191831188924</v>
+        <v>-0.54067964867143159</v>
       </c>
       <c r="G20">
         <f t="shared" ca="1" si="1"/>
-        <v>0.23763881461224257</v>
+        <v>-6.519438367929542E-2</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.94933806569807766</v>
+        <v>0.10923607477560404</v>
       </c>
       <c r="B21">
         <f t="shared" ca="1" si="1"/>
-        <v>0.48293789046203739</v>
+        <v>-0.16537966778119984</v>
       </c>
       <c r="C21">
         <f t="shared" ca="1" si="1"/>
-        <v>0.75273285173674487</v>
+        <v>0.61072018549667995</v>
       </c>
       <c r="D21">
         <f t="shared" ca="1" si="1"/>
-        <v>0.69175219667980037</v>
+        <v>-0.32267506974891136</v>
       </c>
       <c r="E21">
         <f t="shared" ca="1" si="1"/>
-        <v>0.18754938954667022</v>
+        <v>0.16047249985488676</v>
       </c>
       <c r="F21">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.14781689561489153</v>
+        <v>-0.14934624814533448</v>
       </c>
       <c r="G21">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.8931735746370435</v>
+        <v>0.91254178200206315</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" ca="1" si="1"/>
-        <v>0.58851270932560418</v>
+        <v>0.86848193929418382</v>
       </c>
       <c r="B22">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.13284290459340098</v>
+        <v>-0.45417223612236746</v>
       </c>
       <c r="C22">
         <f t="shared" ca="1" si="1"/>
-        <v>6.914223542902076E-2</v>
+        <v>-0.36518095789838223</v>
       </c>
       <c r="D22">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.42298022490843135</v>
+        <v>-0.41039015615664831</v>
       </c>
       <c r="E22">
         <f t="shared" ca="1" si="1"/>
-        <v>0.19619433728169988</v>
+        <v>0.53146803216403837</v>
       </c>
       <c r="F22">
         <f t="shared" ca="1" si="1"/>
-        <v>0.21879939270258419</v>
+        <v>-0.94692134426742491</v>
       </c>
       <c r="G22">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.25725788220958878</v>
+        <v>-0.53106632644814344</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
         <f t="shared" ca="1" si="1"/>
-        <v>1.3235250338074156E-2</v>
+        <v>-0.69365999001896617</v>
       </c>
       <c r="B23">
         <f t="shared" ca="1" si="1"/>
-        <v>-2.9874957522336931E-2</v>
+        <v>0.2988528651439879</v>
       </c>
       <c r="C23">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.68005295943052957</v>
+        <v>-0.98499503175123171</v>
       </c>
       <c r="D23">
         <f t="shared" ca="1" si="1"/>
-        <v>0.94867968422605831</v>
+        <v>-0.60149134256563763</v>
       </c>
       <c r="E23">
         <f t="shared" ca="1" si="1"/>
-        <v>0.67263143087269217</v>
+        <v>-0.79151235541498655</v>
       </c>
       <c r="F23">
         <f t="shared" ca="1" si="1"/>
-        <v>0.54685903755013077</v>
+        <v>0.14916612848280009</v>
       </c>
       <c r="G23">
         <f t="shared" ca="1" si="1"/>
-        <v>0.72588687535821861</v>
+        <v>7.9392490927297166E-2</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" ca="1" si="1"/>
-        <v>0.16753350601508776</v>
+        <v>-6.6033770247493795E-2</v>
       </c>
       <c r="B24">
         <f t="shared" ca="1" si="1"/>
-        <v>4.2387290299308766E-2</v>
+        <v>-0.96349644484497898</v>
       </c>
       <c r="C24">
         <f t="shared" ca="1" si="1"/>
-        <v>0.89654855532222588</v>
+        <v>-0.10309173030370089</v>
       </c>
       <c r="D24">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.94222027454201629</v>
+        <v>0.36558748150190268</v>
       </c>
       <c r="E24">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.7225854377939338</v>
+        <v>0.62606186619245219</v>
       </c>
       <c r="F24">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.62341114413376864</v>
+        <v>-0.391379996382476</v>
       </c>
       <c r="G24">
         <f t="shared" ca="1" si="1"/>
-        <v>0.90865609503295319</v>
+        <v>0.49070967179405489</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.69609323867811157</v>
+        <v>-0.56415676799810432</v>
       </c>
       <c r="B25">
         <f t="shared" ca="1" si="1"/>
-        <v>0.18270559817448828</v>
+        <v>-0.77797127382507192</v>
       </c>
       <c r="C25">
         <f t="shared" ca="1" si="1"/>
-        <v>0.31204503880340262</v>
+        <v>-0.33028217423988471</v>
       </c>
       <c r="D25">
         <f t="shared" ca="1" si="1"/>
-        <v>-1.5969211843896547E-2</v>
+        <v>0.46797174208418024</v>
       </c>
       <c r="E25">
         <f t="shared" ca="1" si="1"/>
-        <v>0.56240633636717852</v>
+        <v>-0.37503933871421125</v>
       </c>
       <c r="F25">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.63567513945546339</v>
+        <v>-0.46569282634824116</v>
       </c>
       <c r="G25">
         <f t="shared" ca="1" si="1"/>
-        <v>0.54197296141876339</v>
+        <v>-0.45779101917670006</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
         <f t="shared" ca="1" si="1"/>
-        <v>0.83499250029329763</v>
+        <v>0.34434610697129031</v>
       </c>
       <c r="B26">
         <f t="shared" ca="1" si="1"/>
-        <v>0.71106626326850764</v>
+        <v>-8.5100975364064579E-2</v>
       </c>
       <c r="C26">
         <f t="shared" ca="1" si="1"/>
-        <v>0.99798493107050734</v>
+        <v>-0.2748546884482328</v>
       </c>
       <c r="D26">
         <f t="shared" ca="1" si="1"/>
-        <v>0.2288352190434555</v>
+        <v>-0.61067290434008692</v>
       </c>
       <c r="E26">
         <f t="shared" ca="1" si="1"/>
-        <v>0.50372943578810259</v>
+        <v>7.2557895573355236E-3</v>
       </c>
       <c r="F26">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.39449337163732934</v>
+        <v>-0.32536793236109141</v>
       </c>
       <c r="G26">
         <f t="shared" ca="1" si="1"/>
-        <v>0.12610476672381554</v>
+        <v>0.56273647324028309</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.41699511663433375</v>
+        <v>0.13599782740215227</v>
       </c>
       <c r="B27">
         <f t="shared" ca="1" si="1"/>
-        <v>0.55812038443746803</v>
+        <v>-0.43652705419294757</v>
       </c>
       <c r="C27">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.25527811266966416</v>
+        <v>-5.5178441180383508E-3</v>
       </c>
       <c r="D27">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.39497761459614456</v>
+        <v>0.21306943909547793</v>
       </c>
       <c r="E27">
         <f t="shared" ca="1" si="1"/>
-        <v>0.33341929905109913</v>
+        <v>-0.97768614466978931</v>
       </c>
       <c r="F27">
         <f t="shared" ca="1" si="1"/>
-        <v>4.3944441610756169E-2</v>
+        <v>-0.81034426716032848</v>
       </c>
       <c r="G27">
         <f t="shared" ca="1" si="1"/>
-        <v>0.90163179748747413</v>
+        <v>-0.29049562314194999</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28">
         <f t="shared" ca="1" si="1"/>
-        <v>0.32273732320821891</v>
+        <v>0.93830251651013419</v>
       </c>
       <c r="B28">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.81931486574861578</v>
+        <v>0.83395995264866629</v>
       </c>
       <c r="C28">
         <f t="shared" ca="1" si="1"/>
-        <v>0.68492701391569</v>
+        <v>-0.62797737478925852</v>
       </c>
       <c r="D28">
         <f t="shared" ca="1" si="1"/>
-        <v>0.65936788818412673</v>
+        <v>-0.10947384891253797</v>
       </c>
       <c r="E28">
         <f t="shared" ca="1" si="1"/>
-        <v>8.5554474619112142E-2</v>
+        <v>-0.27400103680327148</v>
       </c>
       <c r="F28">
         <f t="shared" ca="1" si="1"/>
-        <v>0.48164993693141644</v>
+        <v>0.5476875290401364</v>
       </c>
       <c r="G28">
         <f t="shared" ca="1" si="1"/>
-        <v>0.96300065778878641</v>
+        <v>-0.58539754697396384</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.26327782177356585</v>
+        <v>0.45882595869731779</v>
       </c>
       <c r="B29">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.34180214032518519</v>
+        <v>0.49772452040589088</v>
       </c>
       <c r="C29">
         <f t="shared" ca="1" si="1"/>
-        <v>0.90690762846694195</v>
+        <v>-0.11061795108447692</v>
       </c>
       <c r="D29">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.69697087604571828</v>
+        <v>0.88178173309602492</v>
       </c>
       <c r="E29">
         <f t="shared" ca="1" si="1"/>
-        <v>0.47790035815639875</v>
+        <v>-0.85728875099124924</v>
       </c>
       <c r="F29">
         <f t="shared" ca="1" si="1"/>
-        <v>0.82947448877620888</v>
+        <v>0.31592797254213578</v>
       </c>
       <c r="G29">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.25251307586135407</v>
+        <v>-0.87432064175947</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.50122553327125807</v>
+        <v>0.48360105274084719</v>
       </c>
       <c r="B30">
         <f t="shared" ca="1" si="1"/>
-        <v>0.98333264634454287</v>
+        <v>-0.38437239132140388</v>
       </c>
       <c r="C30">
         <f t="shared" ca="1" si="1"/>
-        <v>0.22054777006028581</v>
+        <v>-0.70233192714671877</v>
       </c>
       <c r="D30">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.99983294626832975</v>
+        <v>-0.84453440566654314</v>
       </c>
       <c r="E30">
         <f t="shared" ca="1" si="1"/>
-        <v>0.25977265359675084</v>
+        <v>4.5550092768582573E-2</v>
       </c>
       <c r="F30">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.76368942638572501</v>
+        <v>0.21358216597097135</v>
       </c>
       <c r="G30">
         <f t="shared" ca="1" si="1"/>
-        <v>0.65815803551207597</v>
+        <v>0.37345717739565831</v>
       </c>
     </row>
   </sheetData>

</xml_diff>